<commit_message>
Added Manage Location Test and Manage Delivery Boy Test cases
</commit_message>
<xml_diff>
--- a/ProjectFramework/src/main/resources/TestData.xlsx
+++ b/ProjectFramework/src/main/resources/TestData.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angit\git\ProjectFramework\ProjectFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470F2862-71AC-4266-95A5-149F29F37FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCD7FB5-F408-4799-977C-59EDD4633C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="ManageProductsPage" sheetId="2" r:id="rId2"/>
+    <sheet name="AddOffercode" sheetId="3" r:id="rId3"/>
+    <sheet name="SearchOfferCode" sheetId="4" r:id="rId4"/>
+    <sheet name="EditOfferCode" sheetId="5" r:id="rId5"/>
+    <sheet name="DeleteOfferCode" sheetId="6" r:id="rId6"/>
+    <sheet name="AddLocation" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>admin</t>
   </si>
@@ -43,7 +48,88 @@
     <t>Title</t>
   </si>
   <si>
-    <t>newproducttitle</t>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Combo</t>
+  </si>
+  <si>
+    <t>Cake</t>
+  </si>
+  <si>
+    <t>Weight Value</t>
+  </si>
+  <si>
+    <t>Maximum Quantity Can Order</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>MRP</t>
+  </si>
+  <si>
+    <t>Stock Availability(Kg)</t>
+  </si>
+  <si>
+    <t>Purchase Price</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Brand new cake additions</t>
+  </si>
+  <si>
+    <t>Image Location</t>
+  </si>
+  <si>
+    <t>C:\\Users\\angit\\Downloads\\Desktop\\cake pic.jpg</t>
+  </si>
+  <si>
+    <t>Offer Code</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>T125</t>
+  </si>
+  <si>
+    <t>Offer code T136 description</t>
+  </si>
+  <si>
+    <t>T138</t>
+  </si>
+  <si>
+    <t>Edited description for Offer code T138</t>
+  </si>
+  <si>
+    <t>T140</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Lynch Street</t>
+  </si>
+  <si>
+    <t>Delivery Charge</t>
   </si>
 </sst>
 </file>
@@ -364,7 +450,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,28 +494,284 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{702FBE8E-4D50-4C39-A207-C8D2159C0C0B}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>950</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBA2D77-87B6-4D6F-A7BE-767583ACBDCC}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>500</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCA5EA3-CDEA-4606-9A4E-039313D886FC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24D4182-E2EC-440B-AF69-DCB415F899CE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFCB530-AB34-4FE4-9A34-70B43E3539B1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A541C73-6B52-4802-8C54-94407F056A1F}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>3815</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test cases in manage location and manage delivery boy test
</commit_message>
<xml_diff>
--- a/ProjectFramework/src/main/resources/TestData.xlsx
+++ b/ProjectFramework/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angit\git\ProjectFramework\ProjectFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCD7FB5-F408-4799-977C-59EDD4633C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69F7020-6E17-4D8C-83EF-92F05A2AEE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="EditOfferCode" sheetId="5" r:id="rId5"/>
     <sheet name="DeleteOfferCode" sheetId="6" r:id="rId6"/>
     <sheet name="AddLocation" sheetId="7" r:id="rId7"/>
+    <sheet name="SearchLocation" sheetId="8" r:id="rId8"/>
+    <sheet name="EditDeliveryBoy" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>admin</t>
   </si>
@@ -99,18 +101,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>T125</t>
-  </si>
-  <si>
-    <t>Offer code T136 description</t>
-  </si>
-  <si>
-    <t>T138</t>
-  </si>
-  <si>
-    <t>Edited description for Offer code T138</t>
-  </si>
-  <si>
     <t>T140</t>
   </si>
   <si>
@@ -130,6 +120,33 @@
   </si>
   <si>
     <t>Delivery Charge</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Rolland Gerlach</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Updated address of Rolland Gerlach</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>T146</t>
+  </si>
+  <si>
+    <t>Offer code T146 description</t>
+  </si>
+  <si>
+    <t>Edited description for Offer code T146</t>
+  </si>
+  <si>
+    <t>T156</t>
   </si>
 </sst>
 </file>
@@ -586,7 +603,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +632,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -624,7 +641,7 @@
         <v>500</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -639,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCA5EA3-CDEA-4606-9A4E-039313D886FC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +672,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -668,7 +685,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,10 +706,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>1000</v>
@@ -708,7 +725,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A541C73-6B52-4802-8C54-94407F056A1F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,27 +761,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>3815</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>100</v>
@@ -774,4 +791,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A328976B-755E-4561-AC5D-B3D4C86DB9F0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265C27F4-FB57-4A30-AAEE-B747071361E9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>123458539</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated testng xml with different include methods
</commit_message>
<xml_diff>
--- a/ProjectFramework/src/main/resources/TestData.xlsx
+++ b/ProjectFramework/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angit\git\ProjectFramework\ProjectFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69F7020-6E17-4D8C-83EF-92F05A2AEE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6D7CB2-6356-4F97-8F1E-0B04DC47F5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>admin</t>
   </si>
@@ -140,13 +140,16 @@
     <t>T146</t>
   </si>
   <si>
-    <t>Offer code T146 description</t>
-  </si>
-  <si>
     <t>Edited description for Offer code T146</t>
   </si>
   <si>
     <t>T156</t>
+  </si>
+  <si>
+    <t>T147</t>
+  </si>
+  <si>
+    <t>Offer code T147 description</t>
   </si>
 </sst>
 </file>
@@ -602,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBA2D77-87B6-4D6F-A7BE-767583ACBDCC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,16 +635,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>500</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -656,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BCA5EA3-CDEA-4606-9A4E-039313D886FC}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -672,7 +675,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -685,7 +688,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,7 +712,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>1000</v>

</xml_diff>

<commit_message>
Updated Grouping testng.xml file
</commit_message>
<xml_diff>
--- a/ProjectFramework/src/main/resources/TestData.xlsx
+++ b/ProjectFramework/src/main/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angit\git\ProjectFramework\ProjectFramework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6D7CB2-6356-4F97-8F1E-0B04DC47F5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6C212E-F5A1-42B4-A7F3-1846E0C3FD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBA2D77-87B6-4D6F-A7BE-767583ACBDCC}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A328976B-755E-4561-AC5D-B3D4C86DB9F0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>